<commit_message>
docs: Se realizan cambios en los archivos de la carpeta Normalizacion
</commit_message>
<xml_diff>
--- a/2-Diseño/05-Normalizacion/Proceso de normalización.xlsx
+++ b/2-Diseño/05-Normalizacion/Proceso de normalización.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APRENDIZ\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96F117F9-EBB5-4045-8923-08DFA67CC4B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="64">
   <si>
     <t>No.Documento</t>
   </si>
@@ -187,9 +183,6 @@
     <t>Crr88a#58-07sur</t>
   </si>
   <si>
-    <t>Codigo_usuario</t>
-  </si>
-  <si>
     <t>Perfil</t>
   </si>
   <si>
@@ -208,24 +201,6 @@
     <t>Costos</t>
   </si>
   <si>
-    <t>Codigo_usuario_1</t>
-  </si>
-  <si>
-    <t>Codigo_usuario_2</t>
-  </si>
-  <si>
-    <t>Codigo_usuario_3</t>
-  </si>
-  <si>
-    <t>Codigo_usuario_4</t>
-  </si>
-  <si>
-    <t>Codigo_usuario_5</t>
-  </si>
-  <si>
-    <t>Codigo_usuario_6</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -239,12 +214,15 @@
   </si>
   <si>
     <t>CASOS DE NORMALIZACION N:2</t>
+  </si>
+  <si>
+    <t>No.Documento2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,7 +599,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -731,15 +709,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,22 +769,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -856,6 +810,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Énfasis6" xfId="2" builtinId="51"/>
@@ -863,6 +826,31 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="134">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -878,12 +866,412 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor rgb="FF009999"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF009999"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -963,151 +1351,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1126,114 +1369,10 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1441,42 +1580,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1542,42 +1645,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
@@ -1643,114 +1710,10 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2786,7 +2749,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2825,7 +2788,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3040,7 +3003,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3310,7 +3273,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -3460,7 +3423,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Estilo de tabla 1" pivot="0" count="0"/>
+    <tableStyle name="Estilo de tabla 1" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <colors>
     <mruColors>
@@ -3479,156 +3442,156 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="B22:J26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla6" displayName="Tabla6" ref="B22:J26" headerRowCount="0" totalsRowShown="0" headerRowDxfId="133" dataDxfId="132">
   <tableColumns count="9">
-    <tableColumn id="1" name="Columna1" dataDxfId="131"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="130"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="129"/>
-    <tableColumn id="4" name="Columna4" dataDxfId="128"/>
-    <tableColumn id="5" name="Columna5" dataDxfId="127"/>
-    <tableColumn id="6" name="Columna6" dataDxfId="126"/>
-    <tableColumn id="7" name="Columna7" dataDxfId="125"/>
-    <tableColumn id="8" name="Columna8" dataDxfId="124"/>
-    <tableColumn id="9" name="Columna9" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Columna1" dataDxfId="131"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Columna2" dataDxfId="130"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Columna3" dataDxfId="129"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Columna4" dataDxfId="128"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Columna5" dataDxfId="127"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Columna6" dataDxfId="126"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Columna7" dataDxfId="125"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Columna8" dataDxfId="124"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Columna9" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Tabla111433" displayName="Tabla111433" ref="L44:L50" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
-  <autoFilter ref="L44:L50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabla111433" displayName="Tabla111433" ref="L44:L50" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+  <autoFilter ref="L44:L50" xr:uid="{00000000-0009-0000-0100-000020000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Sede" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Sede" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="33" name="Tabla33" displayName="Tabla33" ref="B59:B65" totalsRowShown="0" headerRowDxfId="47" dataDxfId="45" headerRowBorderDxfId="46" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="B59:B65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabla33" displayName="Tabla33" ref="B59:B65" totalsRowShown="0" headerRowDxfId="13" dataDxfId="14" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="47">
+  <autoFilter ref="B59:B65" xr:uid="{00000000-0009-0000-0100-000021000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Codigo_usuario" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="No.Documento" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="Tabla3336" displayName="Tabla3336" ref="H69:I75" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38" dataCellStyle="Entrada">
-  <autoFilter ref="H69:I75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Tabla3336" displayName="Tabla3336" ref="H69:I75" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43" dataCellStyle="Entrada">
+  <autoFilter ref="H69:I75" xr:uid="{00000000-0009-0000-0100-000023000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Codigo_usuario" dataDxfId="37" dataCellStyle="Entrada"/>
-    <tableColumn id="2" name="No.Documento" dataCellStyle="Entrada"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="No.Documento" dataDxfId="12" dataCellStyle="Entrada"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="No.Documento2" dataCellStyle="Entrada"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="Tabla3338" displayName="Tabla3338" ref="K69:L75" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33" dataCellStyle="Entrada">
-  <autoFilter ref="K69:L75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabla3338" displayName="Tabla3338" ref="K69:L75" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40" totalsRowBorderDxfId="39" dataCellStyle="Entrada">
+  <autoFilter ref="K69:L75" xr:uid="{00000000-0009-0000-0100-000025000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Codigo_usuario" dataDxfId="32" dataCellStyle="Entrada"/>
-    <tableColumn id="2" name="Direccion" dataDxfId="31" dataCellStyle="Entrada"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="No.Documento" dataDxfId="11" dataCellStyle="Entrada"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Direccion" dataDxfId="38" dataCellStyle="Entrada"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="40" name="Tabla911133241" displayName="Tabla911133241" ref="N59:N65" totalsRowShown="0" headerRowDxfId="30" dataDxfId="28" headerRowBorderDxfId="29" tableBorderDxfId="27" totalsRowBorderDxfId="26">
-  <autoFilter ref="N59:N65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Tabla911133241" displayName="Tabla911133241" ref="N59:N65" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="N59:N65" xr:uid="{00000000-0009-0000-0100-000028000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Horario" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Horario" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Tabla911133242" displayName="Tabla911133242" ref="O69:O75" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20" dataCellStyle="Entrada">
-  <autoFilter ref="O69:O75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Tabla911133242" displayName="Tabla911133242" ref="O69:O75" totalsRowShown="0" headerRowDxfId="31" dataDxfId="29" headerRowBorderDxfId="30" tableBorderDxfId="28" totalsRowBorderDxfId="27" dataCellStyle="Entrada">
+  <autoFilter ref="O69:O75" xr:uid="{00000000-0009-0000-0100-000029000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Horario" dataDxfId="19" dataCellStyle="Entrada"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Horario" dataDxfId="26" dataCellStyle="Entrada"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla332" displayName="Tabla332" ref="N69:N75" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="N69:N75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="Tabla332" displayName="Tabla332" ref="N69:N75" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="25">
+  <autoFilter ref="N69:N75" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Codigo_usuario" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="No.Documento" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla3323" displayName="Tabla3323" ref="Q69:R75" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
-  <autoFilter ref="Q69:R75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF10000000}" name="Tabla3323" displayName="Tabla3323" ref="Q69:R75" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <autoFilter ref="Q69:R75" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Codigo_usuario" dataDxfId="7"/>
-    <tableColumn id="2" name="No.Documento" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="No.Documento" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="No.Documento2" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3324" displayName="Tabla3324" ref="W69:W75" totalsRowShown="0" headerRowDxfId="5" dataDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="2" totalsRowBorderDxfId="1">
-  <autoFilter ref="W69:W75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="Tabla3324" displayName="Tabla3324" ref="W69:W75" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="18">
+  <autoFilter ref="W69:W75" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Codigo_usuario" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="No.Documento" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla66" displayName="Tabla66" ref="B34:J38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla66" displayName="Tabla66" ref="B34:J38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="122" dataDxfId="121">
   <tableColumns count="9">
-    <tableColumn id="1" name="Columna1" dataDxfId="120"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="119"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="118"/>
-    <tableColumn id="4" name="Columna4" dataDxfId="117"/>
-    <tableColumn id="5" name="Columna5" dataDxfId="116"/>
-    <tableColumn id="6" name="Columna6" dataDxfId="115"/>
-    <tableColumn id="7" name="Columna7" dataDxfId="114"/>
-    <tableColumn id="8" name="Columna8" dataDxfId="113"/>
-    <tableColumn id="9" name="Columna9" dataDxfId="112"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Columna1" dataDxfId="120"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Columna2" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Columna3" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Columna4" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Columna5" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Columna6" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Columna7" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Columna8" dataDxfId="113"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Columna9" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="B8:H14" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
-  <autoFilter ref="B8:H14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla7" displayName="Tabla7" ref="B8:H14" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+  <autoFilter ref="B8:H14" xr:uid="{00000000-0009-0000-0100-000007000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3638,21 +3601,21 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" name="No.Documento" dataDxfId="109"/>
-    <tableColumn id="2" name="Primer_Nombre" dataDxfId="108"/>
-    <tableColumn id="3" name="Primer_Apellido" dataDxfId="107"/>
-    <tableColumn id="5" name="Fecha_Nacimiento" dataDxfId="106"/>
-    <tableColumn id="6" name="Telefono" dataDxfId="105"/>
-    <tableColumn id="7" name="Email" dataDxfId="104"/>
-    <tableColumn id="8" name="Direccion" dataDxfId="103"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="No.Documento" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Primer_Nombre" dataDxfId="108"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Primer_Apellido" dataDxfId="107"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Fecha_Nacimiento" dataDxfId="106"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Telefono" dataDxfId="105"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Email" dataDxfId="104"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Direccion" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="I8:M14" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101" tableBorderDxfId="99" totalsRowBorderDxfId="98">
-  <autoFilter ref="I8:M14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabla9" displayName="Tabla9" ref="I8:M14" totalsRowShown="0" headerRowDxfId="102" dataDxfId="100" headerRowBorderDxfId="101" tableBorderDxfId="99" totalsRowBorderDxfId="98">
+  <autoFilter ref="I8:M14" xr:uid="{00000000-0009-0000-0100-000009000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3660,89 +3623,89 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sede" dataDxfId="97"/>
-    <tableColumn id="2" name="Horario" dataDxfId="96"/>
-    <tableColumn id="4" name="Perfil" dataDxfId="95"/>
-    <tableColumn id="5" name="Economia" dataDxfId="94"/>
-    <tableColumn id="3" name="Reunion" dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Sede" dataDxfId="97"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Horario" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Perfil" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Economia" dataDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Reunion" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla911" displayName="Tabla911" ref="L20:O26" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
-  <autoFilter ref="L20:O26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabla911" displayName="Tabla911" ref="L20:O26" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89" totalsRowBorderDxfId="88">
+  <autoFilter ref="L20:O26" xr:uid="{00000000-0009-0000-0100-00000A000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Horario" dataDxfId="87"/>
-    <tableColumn id="3" name="Perfil" dataDxfId="86"/>
-    <tableColumn id="4" name="Economia" dataDxfId="85"/>
-    <tableColumn id="2" name="Reunion" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Horario" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Perfil" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Economia" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Reunion" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla11" displayName="Tabla11" ref="K20:K26" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
-  <autoFilter ref="K20:K26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabla11" displayName="Tabla11" ref="K20:K26" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+  <autoFilter ref="K20:K26" xr:uid="{00000000-0009-0000-0100-00000B000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Sede" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Sede" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla91113" displayName="Tabla91113" ref="L32:O38" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
-  <autoFilter ref="L32:O38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabla91113" displayName="Tabla91113" ref="L32:O38" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+  <autoFilter ref="L32:O38" xr:uid="{00000000-0009-0000-0100-00000C000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Horario" dataDxfId="72"/>
-    <tableColumn id="2" name="Perfil" dataDxfId="71"/>
-    <tableColumn id="3" name="Economia" dataDxfId="70"/>
-    <tableColumn id="4" name="Reunion" dataDxfId="69"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Horario" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Perfil" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Economia" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Reunion" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla1114" displayName="Tabla1114" ref="K32:K38" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
-  <autoFilter ref="K32:K38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabla1114" displayName="Tabla1114" ref="K32:K38" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+  <autoFilter ref="K32:K38" xr:uid="{00000000-0009-0000-0100-00000D000000}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" name="Sede" dataDxfId="63"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Sede" dataDxfId="63"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tabla9111332" displayName="Tabla9111332" ref="M44:P50" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="58">
-  <autoFilter ref="M44:P50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabla9111332" displayName="Tabla9111332" ref="M44:P50" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+  <autoFilter ref="M44:P50" xr:uid="{00000000-0009-0000-0100-00001F000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" name="Horario" dataDxfId="57"/>
-    <tableColumn id="2" name="Perfil" dataDxfId="56"/>
-    <tableColumn id="3" name="Economia" dataDxfId="55"/>
-    <tableColumn id="4" name="Reunion" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Horario" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Perfil" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Economia" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Reunion" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4010,11 +3973,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:X80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="V45" sqref="V45"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="W69" sqref="W69:W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,8 +4012,8 @@
       <c r="B6" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
       <c r="E6" s="25"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -4082,13 +4045,13 @@
         <v>39</v>
       </c>
       <c r="K8" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="74" t="s">
-        <v>67</v>
+      <c r="M8" s="66" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -4120,13 +4083,13 @@
         <v>41</v>
       </c>
       <c r="K9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="M9" s="73" t="s">
-        <v>68</v>
+      <c r="M9" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -4158,13 +4121,13 @@
         <v>45</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M10" s="73" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="M10" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -4196,13 +4159,13 @@
         <v>42</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="73" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="M11" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -4234,13 +4197,13 @@
         <v>43</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M12" s="73" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="M12" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -4272,13 +4235,13 @@
         <v>44</v>
       </c>
       <c r="K13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="M13" s="73" t="s">
-        <v>68</v>
+      <c r="M13" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -4310,13 +4273,13 @@
         <v>40</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="73" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="M14" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:15" ht="30" x14ac:dyDescent="0.4">
@@ -4359,13 +4322,13 @@
         <v>39</v>
       </c>
       <c r="M20" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="N20" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="O20" s="74" t="s">
-        <v>67</v>
+      <c r="O20" s="66" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -4403,13 +4366,13 @@
         <v>41</v>
       </c>
       <c r="M21" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N21" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="N21" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="O21" s="73" t="s">
-        <v>68</v>
+      <c r="O21" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -4447,13 +4410,13 @@
         <v>45</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N22" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="73" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="O22" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -4491,13 +4454,13 @@
         <v>42</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N23" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="O23" s="73" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="O23" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -4535,13 +4498,13 @@
         <v>43</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N24" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="O24" s="73" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="O24" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -4579,13 +4542,13 @@
         <v>44</v>
       </c>
       <c r="M25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N25" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="N25" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="O25" s="73" t="s">
-        <v>68</v>
+      <c r="O25" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
@@ -4623,20 +4586,20 @@
         <v>40</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N26" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="O26" s="73" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="O26" s="65" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="30" x14ac:dyDescent="0.4">
-      <c r="B30" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="81"/>
+      <c r="B30" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="73"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
@@ -4672,14 +4635,14 @@
       <c r="L32" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="M32" s="53" t="s">
+      <c r="M32" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="N32" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="N32" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="O32" s="78" t="s">
-        <v>67</v>
+      <c r="O32" s="70" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
@@ -4713,17 +4676,17 @@
       <c r="K33" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="L33" s="54" t="s">
+      <c r="L33" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="M33" s="55" t="s">
+      <c r="M33" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N33" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="N33" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="O33" s="76" t="s">
-        <v>68</v>
+      <c r="O33" s="68" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
@@ -4757,17 +4720,17 @@
       <c r="K34" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="L34" s="55" t="s">
+      <c r="L34" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="M34" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="N34" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="O34" s="75" t="s">
-        <v>68</v>
+      <c r="M34" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N34" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="O34" s="67" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
@@ -4801,17 +4764,17 @@
       <c r="K35" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="L35" s="55" t="s">
+      <c r="L35" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="M35" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="N35" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="O35" s="75" t="s">
-        <v>68</v>
+      <c r="M35" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N35" s="52" t="s">
+        <v>56</v>
+      </c>
+      <c r="O35" s="67" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
@@ -4845,17 +4808,17 @@
       <c r="K36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="L36" s="55" t="s">
+      <c r="L36" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="M36" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="N36" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="O36" s="75" t="s">
-        <v>68</v>
+      <c r="M36" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N36" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="O36" s="67" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
@@ -4889,17 +4852,17 @@
       <c r="K37" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="L37" s="55" t="s">
+      <c r="L37" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="M37" s="55" t="s">
+      <c r="M37" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N37" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="N37" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="O37" s="75" t="s">
-        <v>68</v>
+      <c r="O37" s="67" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
@@ -4933,17 +4896,17 @@
       <c r="K38" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L38" s="55" t="s">
+      <c r="L38" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="M38" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="N38" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="O38" s="77" t="s">
-        <v>68</v>
+      <c r="M38" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="N38" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="O38" s="69" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.25">
@@ -4994,14 +4957,14 @@
       <c r="M44" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="N44" s="52" t="s">
+      <c r="N44" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="O44" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="O44" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="P44" s="74" t="s">
-        <v>67</v>
+      <c r="P44" s="66" t="s">
+        <v>60</v>
       </c>
       <c r="R44" s="28" t="s">
         <v>0</v>
@@ -5041,22 +5004,22 @@
       <c r="L45" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="M45" s="56" t="s">
+      <c r="M45" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="N45" s="55" t="s">
+      <c r="N45" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="O45" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="O45" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="P45" s="76" t="s">
-        <v>68</v>
-      </c>
-      <c r="R45" s="43">
+      <c r="P45" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="R45" s="40">
         <v>1001201058</v>
       </c>
-      <c r="S45" s="43" t="s">
+      <c r="S45" s="40" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5091,22 +5054,22 @@
       <c r="L46" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="M46" s="58" t="s">
+      <c r="M46" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="N46" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="O46" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="P46" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="R46" s="43">
+      <c r="N46" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="O46" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="P46" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="R46" s="40">
         <v>1001331816</v>
       </c>
-      <c r="S46" s="43" t="s">
+      <c r="S46" s="40" t="s">
         <v>19</v>
       </c>
     </row>
@@ -5141,22 +5104,22 @@
       <c r="L47" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M47" s="58" t="s">
+      <c r="M47" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="N47" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="O47" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="P47" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="R47" s="43">
+      <c r="N47" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="O47" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="P47" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="R47" s="40">
         <v>1022382612</v>
       </c>
-      <c r="S47" s="44" t="s">
+      <c r="S47" s="41" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5191,22 +5154,22 @@
       <c r="L48" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="M48" s="58" t="s">
+      <c r="M48" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="N48" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="O48" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="P48" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="R48" s="43">
+      <c r="N48" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="O48" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="P48" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="R48" s="40">
         <v>1030596457</v>
       </c>
-      <c r="S48" s="43" t="s">
+      <c r="S48" s="40" t="s">
         <v>51</v>
       </c>
     </row>
@@ -5241,22 +5204,22 @@
       <c r="L49" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M49" s="58" t="s">
+      <c r="M49" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="N49" s="55" t="s">
+      <c r="N49" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="O49" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="O49" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="P49" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="R49" s="43">
+      <c r="P49" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="R49" s="40">
         <v>52191527</v>
       </c>
-      <c r="S49" s="44" t="s">
+      <c r="S49" s="41" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5291,22 +5254,22 @@
       <c r="L50" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M50" s="59" t="s">
+      <c r="M50" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="N50" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="O50" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="P50" s="77" t="s">
-        <v>68</v>
-      </c>
-      <c r="R50" s="43">
+      <c r="N50" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="O50" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="P50" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="R50" s="40">
         <v>79126086</v>
       </c>
-      <c r="S50" s="44" t="s">
+      <c r="S50" s="41" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5316,28 +5279,28 @@
       </c>
     </row>
     <row r="58" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B58" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="K58" s="72" t="s">
+      <c r="B58" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="K58" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="N58" s="72" t="s">
+      <c r="N58" s="64" t="s">
         <v>39</v>
       </c>
-      <c r="P58" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="R58" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="T58" s="72" t="s">
-        <v>67</v>
+      <c r="P58" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="R58" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="T58" s="64" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B59" s="40" t="s">
-        <v>52</v>
+      <c r="B59" s="75" t="s">
+        <v>0</v>
       </c>
       <c r="C59" s="37" t="s">
         <v>1</v>
@@ -5372,16 +5335,16 @@
       <c r="P59" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="R59" s="71" t="s">
-        <v>53</v>
+      <c r="R59" s="63" t="s">
+        <v>52</v>
       </c>
       <c r="T59" s="21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B60" s="39" t="s">
-        <v>59</v>
+      <c r="B60" s="74">
+        <v>1001201058</v>
       </c>
       <c r="C60" s="38" t="s">
         <v>9</v>
@@ -5404,10 +5367,10 @@
       <c r="I60" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K60" s="45" t="s">
+      <c r="K60" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="L60" s="49" t="s">
+      <c r="L60" s="46" t="s">
         <v>36</v>
       </c>
       <c r="N60" s="17" t="s">
@@ -5416,16 +5379,16 @@
       <c r="P60" s="26">
         <v>1001201058</v>
       </c>
-      <c r="R60" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="T60" s="55" t="s">
-        <v>68</v>
+      <c r="R60" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="T60" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B61" s="39" t="s">
-        <v>60</v>
+      <c r="B61" s="74">
+        <v>1001331816</v>
       </c>
       <c r="C61" s="38" t="s">
         <v>14</v>
@@ -5448,10 +5411,10 @@
       <c r="I61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K61" s="45" t="s">
+      <c r="K61" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="L61" s="49" t="s">
+      <c r="L61" s="46" t="s">
         <v>37</v>
       </c>
       <c r="N61" s="18" t="s">
@@ -5460,16 +5423,16 @@
       <c r="P61" s="26">
         <v>1001331816</v>
       </c>
-      <c r="R61" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="T61" s="55" t="s">
-        <v>68</v>
+      <c r="R61" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="T61" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B62" s="39" t="s">
-        <v>61</v>
+      <c r="B62" s="74">
+        <v>1022382612</v>
       </c>
       <c r="C62" s="38" t="s">
         <v>21</v>
@@ -5492,10 +5455,10 @@
       <c r="I62" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K62" s="46" t="s">
+      <c r="K62" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="L62" s="49" t="s">
+      <c r="L62" s="46" t="s">
         <v>38</v>
       </c>
       <c r="N62" s="18" t="s">
@@ -5504,16 +5467,16 @@
       <c r="P62" s="26">
         <v>1022382612</v>
       </c>
-      <c r="R62" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="T62" s="55" t="s">
-        <v>68</v>
+      <c r="R62" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="T62" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B63" s="39" t="s">
-        <v>62</v>
+      <c r="B63" s="74">
+        <v>1030596457</v>
       </c>
       <c r="C63" s="38" t="s">
         <v>25</v>
@@ -5536,10 +5499,10 @@
       <c r="I63" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K63" s="47" t="s">
+      <c r="K63" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="L63" s="49" t="s">
+      <c r="L63" s="46" t="s">
         <v>37</v>
       </c>
       <c r="N63" s="18" t="s">
@@ -5548,16 +5511,16 @@
       <c r="P63" s="26">
         <v>1030596457</v>
       </c>
-      <c r="R63" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="T63" s="55" t="s">
-        <v>68</v>
+      <c r="R63" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="T63" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B64" s="39" t="s">
-        <v>63</v>
+      <c r="B64" s="74">
+        <v>52191527</v>
       </c>
       <c r="C64" s="38" t="s">
         <v>13</v>
@@ -5580,10 +5543,10 @@
       <c r="I64" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K64" s="46" t="s">
+      <c r="K64" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="L64" s="48" t="s">
+      <c r="L64" s="45" t="s">
         <v>35</v>
       </c>
       <c r="N64" s="18" t="s">
@@ -5592,16 +5555,16 @@
       <c r="P64" s="26">
         <v>52191527</v>
       </c>
-      <c r="R64" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="T64" s="55" t="s">
-        <v>68</v>
+      <c r="R64" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="T64" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B65" s="41" t="s">
-        <v>64</v>
+      <c r="B65" s="76">
+        <v>79126086</v>
       </c>
       <c r="C65" s="38" t="s">
         <v>29</v>
@@ -5624,10 +5587,10 @@
       <c r="I65" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K65" s="46" t="s">
+      <c r="K65" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="L65" s="48" t="s">
+      <c r="L65" s="45" t="s">
         <v>35</v>
       </c>
       <c r="N65" s="19" t="s">
@@ -5636,277 +5599,277 @@
       <c r="P65" s="26">
         <v>79126086</v>
       </c>
-      <c r="R65" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="T65" s="55" t="s">
-        <v>68</v>
+      <c r="R65" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="T65" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H69" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="I69" s="42" t="s">
+      <c r="H69" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="K69" s="40" t="s">
-        <v>52</v>
+      <c r="I69" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="K69" s="28" t="s">
+        <v>0</v>
       </c>
       <c r="L69" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="N69" s="40" t="s">
-        <v>52</v>
+      <c r="N69" s="75" t="s">
+        <v>0</v>
       </c>
       <c r="O69" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="Q69" s="65" t="s">
+      <c r="Q69" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="R69" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="T69" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="U69" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="R69" s="70" t="s">
+      <c r="W69" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="T69" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="U69" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="W69" s="40" t="s">
-        <v>52</v>
-      </c>
       <c r="X69" s="21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H70" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="I70" s="50">
+      <c r="H70" s="3">
         <v>1001201058</v>
       </c>
-      <c r="K70" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="L70" s="45" t="s">
+      <c r="I70" s="47">
+        <v>1001201058</v>
+      </c>
+      <c r="K70" s="3">
+        <v>1001201058</v>
+      </c>
+      <c r="L70" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="N70" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="O70" s="51" t="s">
+      <c r="N70" s="74">
+        <v>1001201058</v>
+      </c>
+      <c r="O70" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="Q70" s="66" t="s">
-        <v>59</v>
-      </c>
-      <c r="R70" s="68">
+      <c r="Q70" s="3">
         <v>1001201058</v>
       </c>
-      <c r="T70" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="U70" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W70" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="X70" s="55" t="s">
-        <v>68</v>
+      <c r="R70" s="60">
+        <v>1001201058</v>
+      </c>
+      <c r="T70" s="3">
+        <v>1001201058</v>
+      </c>
+      <c r="U70" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W70" s="74">
+        <v>1001201058</v>
+      </c>
+      <c r="X70" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H71" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="I71" s="50">
+      <c r="H71" s="3">
         <v>1001331816</v>
       </c>
-      <c r="K71" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="L71" s="45" t="s">
+      <c r="I71" s="47">
+        <v>1001331816</v>
+      </c>
+      <c r="K71" s="3">
+        <v>1001331816</v>
+      </c>
+      <c r="L71" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="N71" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="O71" s="50" t="s">
+      <c r="N71" s="74">
+        <v>1001331816</v>
+      </c>
+      <c r="O71" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="Q71" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="R71" s="68">
+      <c r="Q71" s="3">
         <v>1001331816</v>
       </c>
-      <c r="T71" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="U71" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W71" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="X71" s="55" t="s">
-        <v>68</v>
+      <c r="R71" s="60">
+        <v>1001331816</v>
+      </c>
+      <c r="T71" s="3">
+        <v>1001331816</v>
+      </c>
+      <c r="U71" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W71" s="74">
+        <v>1001331816</v>
+      </c>
+      <c r="X71" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H72" s="39" t="s">
+      <c r="H72" s="3">
+        <v>1022382612</v>
+      </c>
+      <c r="I72" s="47">
+        <v>1022382612</v>
+      </c>
+      <c r="K72" s="3">
+        <v>1022382612</v>
+      </c>
+      <c r="L72" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="N72" s="74">
+        <v>1022382612</v>
+      </c>
+      <c r="O72" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q72" s="3">
+        <v>1022382612</v>
+      </c>
+      <c r="R72" s="60">
+        <v>1022382612</v>
+      </c>
+      <c r="T72" s="3">
+        <v>1022382612</v>
+      </c>
+      <c r="U72" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W72" s="74">
+        <v>1022382612</v>
+      </c>
+      <c r="X72" s="52" t="s">
         <v>61</v>
-      </c>
-      <c r="I72" s="50">
-        <v>1022382612</v>
-      </c>
-      <c r="K72" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="L72" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="N72" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="O72" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q72" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="R72" s="68">
-        <v>1022382612</v>
-      </c>
-      <c r="T72" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="U72" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W72" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="X72" s="55" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="73" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H73" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="I73" s="50">
+      <c r="H73" s="3">
         <v>1030596457</v>
       </c>
-      <c r="K73" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="L73" s="47" t="s">
+      <c r="I73" s="47">
+        <v>1030596457</v>
+      </c>
+      <c r="K73" s="3">
+        <v>1030596457</v>
+      </c>
+      <c r="L73" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="N73" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="O73" s="50" t="s">
+      <c r="N73" s="74">
+        <v>1030596457</v>
+      </c>
+      <c r="O73" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="Q73" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="R73" s="68">
+      <c r="Q73" s="3">
         <v>1030596457</v>
       </c>
-      <c r="T73" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="U73" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W73" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="X73" s="55" t="s">
-        <v>68</v>
+      <c r="R73" s="60">
+        <v>1030596457</v>
+      </c>
+      <c r="T73" s="3">
+        <v>1030596457</v>
+      </c>
+      <c r="U73" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W73" s="74">
+        <v>1030596457</v>
+      </c>
+      <c r="X73" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H74" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="I74" s="50">
+      <c r="H74" s="3">
         <v>52191527</v>
       </c>
-      <c r="K74" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="L74" s="46" t="s">
+      <c r="I74" s="47">
+        <v>52191527</v>
+      </c>
+      <c r="K74" s="3">
+        <v>52191527</v>
+      </c>
+      <c r="L74" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="N74" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="O74" s="50" t="s">
+      <c r="N74" s="74">
+        <v>52191527</v>
+      </c>
+      <c r="O74" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="Q74" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="R74" s="68">
+      <c r="Q74" s="3">
         <v>52191527</v>
       </c>
-      <c r="T74" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="U74" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W74" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="X74" s="55" t="s">
-        <v>68</v>
+      <c r="R74" s="60">
+        <v>52191527</v>
+      </c>
+      <c r="T74" s="3">
+        <v>52191527</v>
+      </c>
+      <c r="U74" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W74" s="74">
+        <v>52191527</v>
+      </c>
+      <c r="X74" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="H75" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="I75" s="50">
+      <c r="H75" s="3">
         <v>79126086</v>
       </c>
-      <c r="K75" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="L75" s="46" t="s">
+      <c r="I75" s="47">
+        <v>79126086</v>
+      </c>
+      <c r="K75" s="3">
+        <v>79126086</v>
+      </c>
+      <c r="L75" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="N75" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="O75" s="50" t="s">
+      <c r="N75" s="76">
+        <v>79126086</v>
+      </c>
+      <c r="O75" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="Q75" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="R75" s="69">
+      <c r="Q75" s="3">
         <v>79126086</v>
       </c>
-      <c r="T75" s="63" t="s">
-        <v>64</v>
-      </c>
-      <c r="U75" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="W75" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="X75" s="55" t="s">
-        <v>68</v>
+      <c r="R75" s="61">
+        <v>79126086</v>
+      </c>
+      <c r="T75" s="3">
+        <v>79126086</v>
+      </c>
+      <c r="U75" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="W75" s="76">
+        <v>79126086</v>
+      </c>
+      <c r="X75" s="52" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="2:24" x14ac:dyDescent="0.25">
@@ -5920,36 +5883,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I21" r:id="rId1"/>
-    <hyperlink ref="I22" r:id="rId2"/>
-    <hyperlink ref="I23" r:id="rId3"/>
-    <hyperlink ref="I24" r:id="rId4"/>
-    <hyperlink ref="I25" r:id="rId5"/>
-    <hyperlink ref="I26" r:id="rId6"/>
-    <hyperlink ref="I33" r:id="rId7"/>
-    <hyperlink ref="I34" r:id="rId8"/>
-    <hyperlink ref="I35" r:id="rId9"/>
-    <hyperlink ref="I36" r:id="rId10"/>
-    <hyperlink ref="I37" r:id="rId11"/>
-    <hyperlink ref="I38" r:id="rId12"/>
-    <hyperlink ref="G9" r:id="rId13"/>
-    <hyperlink ref="G10" r:id="rId14"/>
-    <hyperlink ref="G11" r:id="rId15"/>
-    <hyperlink ref="G12" r:id="rId16"/>
-    <hyperlink ref="G13" r:id="rId17"/>
-    <hyperlink ref="G14" r:id="rId18"/>
-    <hyperlink ref="J45" r:id="rId19"/>
-    <hyperlink ref="J46" r:id="rId20"/>
-    <hyperlink ref="J47" r:id="rId21"/>
-    <hyperlink ref="J48" r:id="rId22"/>
-    <hyperlink ref="J49" r:id="rId23"/>
-    <hyperlink ref="J50" r:id="rId24"/>
-    <hyperlink ref="I60" r:id="rId25"/>
-    <hyperlink ref="I61" r:id="rId26"/>
-    <hyperlink ref="I62" r:id="rId27"/>
-    <hyperlink ref="I63" r:id="rId28"/>
-    <hyperlink ref="I64" r:id="rId29"/>
-    <hyperlink ref="I65" r:id="rId30"/>
+    <hyperlink ref="I21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="I22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="I23" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I24" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="I25" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I26" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="I33" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="I34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I35" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="I36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="I37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="I38" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G9" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J45" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J46" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J47" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J48" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J49" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J50" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="I60" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="I61" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="I62" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="I63" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="I64" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="I65" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>

</xml_diff>